<commit_message>
Added Fragen 31_03.txt Changed AnforderungenFinalxlsx.xlsx
</commit_message>
<xml_diff>
--- a/AnforderungenFinalxlsx.xlsx
+++ b/AnforderungenFinalxlsx.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias Reckmeyer\Documents\Git\x-share\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="20160" windowHeight="7740"/>
   </bookViews>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="158">
   <si>
     <t>Produkt verleihen</t>
   </si>
@@ -151,9 +156,6 @@
     <t>Benutzer löschen</t>
   </si>
   <si>
-    <t>Produkte löschen</t>
-  </si>
-  <si>
     <t>Produkt verwalten</t>
   </si>
   <si>
@@ -488,13 +490,19 @@
   </si>
   <si>
     <t>Endanwendung verwalten</t>
+  </si>
+  <si>
+    <t>Produkte entfernen</t>
+  </si>
+  <si>
+    <t>Produkte suchen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -653,9 +661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -693,9 +701,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,9 +735,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,9 +770,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -936,14 +946,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="2" customWidth="1"/>
@@ -955,29 +965,29 @@
     <col min="8" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45.75" customHeight="1">
+    <row r="1" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -989,133 +999,133 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1">
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1">
+    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1">
+    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="25.5" customHeight="1">
+    <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1125,7 +1135,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -1137,79 +1147,79 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="45" customHeight="1">
+    <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>144</v>
-      </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1219,7 +1229,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="25.5" customHeight="1">
+    <row r="17" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>4</v>
       </c>
@@ -1231,79 +1241,79 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="60" customHeight="1">
+    <row r="20" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1313,7 +1323,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="92.25" customHeight="1">
+    <row r="23" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>2</v>
       </c>
@@ -1321,17 +1331,17 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1341,7 +1351,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1351,7 +1361,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="25.5" customHeight="1">
+    <row r="26" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>5</v>
       </c>
@@ -1363,79 +1373,79 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="60" customHeight="1">
+    <row r="27" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="38.25" customHeight="1">
+    <row r="29" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="25.5" customHeight="1">
+    <row r="30" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1">
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1445,7 +1455,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="25.5" customHeight="1">
+    <row r="32" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -1457,25 +1467,25 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="62.25" customHeight="1">
+    <row r="33" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="39.75" customHeight="1">
+    <row r="34" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
         <v>27</v>
@@ -1484,14 +1494,14 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1501,7 +1511,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>8</v>
       </c>
@@ -1513,43 +1523,43 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="25.5" customHeight="1">
+    <row r="37" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="43.5" customHeight="1">
+    <row r="38" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1559,7 +1569,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>7</v>
       </c>
@@ -1571,25 +1581,25 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="45" customHeight="1">
+    <row r="41" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1">
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1599,7 +1609,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1">
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>6</v>
       </c>
@@ -1611,43 +1621,43 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1">
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1657,7 +1667,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1">
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>1</v>
       </c>
@@ -1669,43 +1679,43 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="25.5" customHeight="1">
+    <row r="48" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="38.25" customHeight="1">
+    <row r="49" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
       <c r="B49" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="12.75" customHeight="1">
+    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1715,9 +1725,9 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" ht="12.75" customHeight="1">
+    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1727,79 +1737,79 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="45" customHeight="1">
+    <row r="53" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
       <c r="B53" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="45" customHeight="1">
+    <row r="54" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
       <c r="B54" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="B55" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="12.75" customHeight="1">
+    <row r="56" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1809,7 +1819,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" ht="25.5" customHeight="1">
+    <row r="57" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>9</v>
       </c>
@@ -1821,61 +1831,61 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" ht="27" customHeight="1">
+    <row r="58" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9"/>
       <c r="B58" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
       <c r="B59" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" ht="12.75" customHeight="1">
+    <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1885,7 +1895,7 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" ht="12.75" customHeight="1">
+    <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>11</v>
       </c>
@@ -1897,25 +1907,25 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="B63" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" ht="12.75" customHeight="1">
+    <row r="64" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1925,7 +1935,7 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" ht="38.25" customHeight="1">
+    <row r="65" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>12</v>
       </c>
@@ -1937,25 +1947,25 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" ht="80.45" customHeight="1">
+    <row r="66" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G66" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" ht="12.75" customHeight="1">
+    <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1965,7 +1975,7 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" ht="12.75" customHeight="1">
+    <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>10</v>
       </c>
@@ -1977,39 +1987,39 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="9"/>
       <c r="B69" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" ht="135" customHeight="1">
+    <row r="70" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="5"/>
       <c r="G70" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" ht="12.75" customHeight="1">
+    <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2019,7 +2029,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1">
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>13</v>
       </c>
@@ -2031,43 +2041,43 @@
       <c r="G72" s="4"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" ht="51" customHeight="1">
+    <row r="73" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9"/>
       <c r="B73" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" ht="25.5" customHeight="1">
+    <row r="74" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" ht="12.75" customHeight="1">
+    <row r="75" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -2077,9 +2087,9 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" ht="12.75" customHeight="1">
+    <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -2087,39 +2097,39 @@
       <c r="E76" s="3"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" ht="38.25" customHeight="1">
+    <row r="77" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9"/>
       <c r="B77" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" ht="25.5" customHeight="1">
+    <row r="78" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="3" t="s">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -2129,9 +2139,9 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
     </row>
-    <row r="80" spans="1:8" ht="12.75" customHeight="1">
+    <row r="80" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -2141,21 +2151,21 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="8"/>
       <c r="B81" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G81" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="H81" s="3"/>
     </row>

</xml_diff>